<commit_message>
commit lib files from simulink project
</commit_message>
<xml_diff>
--- a/cm/UnitFolder/interfaceUnit填写指南.xlsx
+++ b/cm/UnitFolder/interfaceUnit填写指南.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhoutinglin\Documents\1_MyDoc\Doc2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhoutinglin\MATLAB\newEMS.git\cm\UnitFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C2F043-9636-4A95-B37D-EB4EB21E6ACB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D77FEA8-893C-4F5B-BC35-36FDEF9B4F47}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总则" sheetId="9" r:id="rId1"/>
@@ -1096,10 +1096,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>请不要更改表格任何格式，包括字体、字号、单元格对齐方式、行高等，仅填写内容。对于从其它地方复制过来的内容，仅保留源值即可。对于列宽，出于显示需要，可以适当调整。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[1 30]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1198,6 +1194,10 @@
   </si>
   <si>
     <t>做出解释；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请不要更改表格任何格式，包括字体、字号、单元格对齐方式、行高等，仅填写内容。对于从其它地方复制过来的内容，仅保留源值，不要保留格式。对于列宽，出于显示需要，可以适当调整。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1783,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F83BF1-B029-45B1-86DA-A0028B373ECD}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="33" x14ac:dyDescent="0.15">
@@ -1815,7 +1815,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.15">
@@ -1823,7 +1823,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="33" x14ac:dyDescent="0.15">
@@ -1839,7 +1839,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="33" x14ac:dyDescent="0.15">
@@ -1847,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
@@ -1863,7 +1863,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2290,16 +2290,16 @@
         <v>255</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2605,22 +2605,22 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2715,7 +2715,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>